<commit_message>
Fix fairness solver for marimo
</commit_message>
<xml_diff>
--- a/apps/ngs-fairness-solver-files/ngs_fairness_solver_input_tmpl.xlsx
+++ b/apps/ngs-fairness-solver-files/ngs_fairness_solver_input_tmpl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rng/ownCloud/Documents/AO/##PROJ/NGS/NGS_Fairness_Solver/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rng/Documents/VSCode_Workspace/marimo_ngs/apps/ngs-fairness-solver-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F007B677-7A81-9643-AB4C-49AC5DAE16DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC8E369-9E96-D744-B3A2-7B1F4425DA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17100" yWindow="780" windowWidth="17100" windowHeight="20040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17100" yWindow="780" windowWidth="17100" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Periods" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -580,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865BE05-1083-4CC1-9803-356C528EE390}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>